<commit_message>
feat: implement excel reading
</commit_message>
<xml_diff>
--- a/business_rules.xlsx
+++ b/business_rules.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdobi/Documents/private/business-rule-parser/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdobi/Documents/private/rule-engine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BE244B-1E0A-454A-9FBB-4A14A3CE466C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B247AB-518B-8644-B182-160982179F24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{62279B5E-BE8D-DD44-8B69-63491B5CFE15}"/>
+    <workbookView xWindow="33600" yWindow="-2480" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{62279B5E-BE8D-DD44-8B69-63491B5CFE15}"/>
   </bookViews>
   <sheets>
-    <sheet name="Rules" sheetId="1" r:id="rId1"/>
+    <sheet name="Entities" sheetId="2" r:id="rId1"/>
+    <sheet name="Rules" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
   <si>
     <t>Minimum Age Rule</t>
   </si>
@@ -51,26 +52,142 @@
     <t>Company</t>
   </si>
   <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>Operator</t>
-  </si>
-  <si>
-    <t>&gt;</t>
-  </si>
-  <si>
-    <t>Value</t>
+    <t>Entity Name</t>
+  </si>
+  <si>
+    <t>Property Name</t>
+  </si>
+  <si>
+    <t>Property Type</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>registrationDate</t>
+  </si>
+  <si>
+    <t>legalForm</t>
+  </si>
+  <si>
+    <t>sbiCodes</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>financialData</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>town</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>FinancialData</t>
+  </si>
+  <si>
+    <t>totalAssets</t>
+  </si>
+  <si>
+    <t>equity</t>
+  </si>
+  <si>
+    <t>revenue</t>
+  </si>
+  <si>
+    <t>profit</t>
+  </si>
+  <si>
+    <t>ebitda</t>
+  </si>
+  <si>
+    <t>minimum</t>
+  </si>
+  <si>
+    <t>maximum</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>LocalDate</t>
+  </si>
+  <si>
+    <t>Collection&lt;String&gt;</t>
+  </si>
+  <si>
+    <t>Int</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>after</t>
+  </si>
+  <si>
+    <t>Operator name</t>
+  </si>
+  <si>
+    <t>Operator type</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Legal Form Rule</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>Value(s)</t>
+  </si>
+  <si>
+    <t>Ltd;Corp;Llp;Plc</t>
+  </si>
+  <si>
+    <t>collection/string</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>gt</t>
+  </si>
+  <si>
+    <t>Minimum Revenue Rule</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -96,8 +213,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,53 +530,304 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C52B3BD0-C472-A94C-9EC5-8142839091C8}">
-  <dimension ref="B2:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84FC577A-F4F2-0D44-9436-EC3761CFF01E}">
+  <dimension ref="B2:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.1640625" customWidth="1"/>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
-        <v>8</v>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C52B3BD0-C472-A94C-9EC5-8142839091C8}">
+  <dimension ref="B2:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3">
-        <v>9</v>
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="2">
+        <v>43466</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5">
+        <v>100000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: generate model objects
</commit_message>
<xml_diff>
--- a/business_rules.xlsx
+++ b/business_rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdobi/Documents/private/rule-engine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B247AB-518B-8644-B182-160982179F24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2571DA25-7D43-2741-BB9A-DC89682F3FA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="-2480" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{62279B5E-BE8D-DD44-8B69-63491B5CFE15}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{62279B5E-BE8D-DD44-8B69-63491B5CFE15}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
   <si>
     <t>Minimum Age Rule</t>
   </si>
@@ -118,9 +118,6 @@
     <t>String</t>
   </si>
   <si>
-    <t>LocalDate</t>
-  </si>
-  <si>
     <t>Collection&lt;String&gt;</t>
   </si>
   <si>
@@ -164,6 +161,12 @@
   </si>
   <si>
     <t>Minimum Revenue Rule</t>
+  </si>
+  <si>
+    <t>AddressDTO</t>
+  </si>
+  <si>
+    <t>FinancialDataDTO</t>
   </si>
 </sst>
 </file>
@@ -533,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84FC577A-F4F2-0D44-9436-EC3761CFF01E}">
   <dimension ref="B2:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -580,7 +583,7 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
@@ -602,7 +605,7 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
@@ -613,7 +616,7 @@
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
@@ -624,7 +627,7 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
@@ -668,7 +671,7 @@
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
@@ -679,7 +682,7 @@
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
@@ -690,7 +693,7 @@
         <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
@@ -701,7 +704,7 @@
         <v>21</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
@@ -712,7 +715,7 @@
         <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
@@ -723,7 +726,7 @@
         <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -736,7 +739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C52B3BD0-C472-A94C-9EC5-8142839091C8}">
   <dimension ref="B2:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
@@ -761,13 +764,13 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
@@ -781,10 +784,10 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3" s="2">
         <v>43466</v>
@@ -792,7 +795,7 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -801,18 +804,18 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -821,10 +824,10 @@
         <v>21</v>
       </c>
       <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
         <v>40</v>
-      </c>
-      <c r="F5" t="s">
-        <v>41</v>
       </c>
       <c r="G5">
         <v>100000</v>

</xml_diff>

<commit_message>
feat: first working rule execution
</commit_message>
<xml_diff>
--- a/business_rules.xlsx
+++ b/business_rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdobi/Documents/private/rule-engine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF50DBE-6388-2D4E-965F-4530F762992C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4BDBD3-292F-3F40-AA38-0E724CD96F02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{62279B5E-BE8D-DD44-8B69-63491B5CFE15}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{62279B5E-BE8D-DD44-8B69-63491B5CFE15}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="2" r:id="rId1"/>
@@ -530,7 +530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84FC577A-F4F2-0D44-9436-EC3761CFF01E}">
   <dimension ref="B2:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -733,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C52B3BD0-C472-A94C-9EC5-8142839091C8}">
   <dimension ref="B2:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
feat: inline entity hierarchy on event
</commit_message>
<xml_diff>
--- a/business_rules.xlsx
+++ b/business_rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdobi/Documents/private/rule-engine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4BDBD3-292F-3F40-AA38-0E724CD96F02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54CCE77-637A-604C-9E18-27827EE39E16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{62279B5E-BE8D-DD44-8B69-63491B5CFE15}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{62279B5E-BE8D-DD44-8B69-63491B5CFE15}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
   <si>
     <t>Minimum Age Rule</t>
   </si>
@@ -528,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84FC577A-F4F2-0D44-9436-EC3761CFF01E}">
-  <dimension ref="B2:F17"/>
+  <dimension ref="B2:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -723,6 +723,17 @@
         <v>29</v>
       </c>
     </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -733,7 +744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C52B3BD0-C472-A94C-9EC5-8142839091C8}">
   <dimension ref="B2:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>

</xml_diff>